<commit_message>
Sistema CR300 Tataouine añadido. Peregiles I -> Notos
</commit_message>
<xml_diff>
--- a/control_emails.xlsx
+++ b/control_emails.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO87"/>
+  <dimension ref="A1:AO88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3019,17 +3019,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Czempin</t>
+          <t>CR300 Tataouine</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>WLS72112</t>
+          <t>CR300 Tataouine</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -3051,7 +3051,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
@@ -3150,7 +3150,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Emsbueren</t>
+          <t>Czempin</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>WLS72103</t>
+          <t>WLS72112</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -3281,27 +3281,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Eolo Austral 1: mag 2</t>
+          <t>Emsbueren</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Eolo_Austral-1</t>
+          <t>WLS72103</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
         <v>1</v>
@@ -3376,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="AE22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF22" t="n">
         <v>1</v>
@@ -3412,27 +3412,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ERAL-A</t>
+          <t>Eolo Austral 1: mag 2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>WLS72030</t>
+          <t>Eolo_Austral-1</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
@@ -3507,7 +3507,7 @@
         <v>1</v>
       </c>
       <c r="AE23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF23" t="n">
         <v>1</v>
@@ -3543,7 +3543,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ERO_1D</t>
+          <t>ERAL-A</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -3553,138 +3553,138 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>WLS71514</t>
+          <t>WLS72030</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ESM1</t>
+          <t>ERO_1D</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ESM1</t>
+          <t>WLS71514</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -3805,7 +3805,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ESM2</t>
+          <t>ESM1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3815,7 +3815,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ESM2</t>
+          <t>ESM1</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -3936,138 +3936,138 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FIA2-B</t>
+          <t>ESM2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>WLS72026</t>
+          <t>ESM2</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Fortmülher</t>
+          <t>FIA2-B</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -4077,7 +4077,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>WLS72101</t>
+          <t>WLS72026</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -4198,7 +4198,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ILLA-A</t>
+          <t>Fortmülher</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>WLS72027</t>
+          <t>WLS72101</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -4329,7 +4329,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Kavelstorf</t>
+          <t>ILLA-A</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>WLS71626</t>
+          <t>WLS72027</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -4460,17 +4460,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Laayoune</t>
+          <t>Kavelstorf</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Laayoune</t>
+          <t>WLS71626</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -4591,17 +4591,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Lagunillas</t>
+          <t>Laayoune</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>estaciones.meteo@dekra-industrial.es</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>LIDAR Lagunillas</t>
+          <t>Laayoune</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -4722,17 +4722,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Lagunillas_2</t>
+          <t>Lagunillas</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>estaciones.meteo@dekra-industrial.es</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>WLS71325</t>
+          <t>LIDAR Lagunillas</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -4853,17 +4853,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Libeccio</t>
+          <t>Lagunillas_2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>estaciones.meteo@dekra-industrial.es</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LIDAR Libeccio</t>
+          <t>WLS71325</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -4984,17 +4984,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Libeccio_2</t>
+          <t>Libeccio</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>estaciones.meteo@dekra-industrial.es</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>WLS72090</t>
+          <t>LIDAR Libeccio</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -5115,17 +5115,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>LJU5</t>
+          <t>Libeccio_2</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LJU5</t>
+          <t>WLS72090</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -5144,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="n">
         <v>1</v>
@@ -5246,7 +5246,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>LJU6</t>
+          <t>LJU5</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -5256,7 +5256,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LJU6</t>
+          <t>LJU5</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -5275,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
         <v>1</v>
@@ -5377,7 +5377,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Los Aguilillos</t>
+          <t>LJU6</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -5387,7 +5387,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>AGUILILLOS</t>
+          <t>LJU6</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -5508,17 +5508,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LUUR-A</t>
+          <t>Los Aguilillos</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>WLS72029</t>
+          <t>AGUILILLOS</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -5639,138 +5639,138 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Magallanes-1</t>
+          <t>LUUR-A</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MAGALLANES-1</t>
+          <t>WLS72029</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Magallanes-2</t>
+          <t>Magallanes-1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -5780,7 +5780,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>MAGALLANES-2</t>
+          <t>MAGALLANES-1</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -5901,148 +5901,148 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Melroeira_Lidar_1</t>
+          <t>Magallanes-2</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>WLS71488</t>
+          <t>MAGALLANES-2</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Melroeira_Lidar_1/Estremoz</t>
+          <t>Melroeira_Lidar_1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>LIDAR Estremoz</t>
+          <t>WLS71488</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -6163,17 +6163,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Montecabeza2_Pos1</t>
+          <t>Melroeira_Lidar_1/Estremoz</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>WLS71630</t>
+          <t>LIDAR Estremoz</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -6294,7 +6294,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MU1P-C</t>
+          <t>Montecabeza2_Pos1</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -6304,7 +6304,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>WLS72060</t>
+          <t>WLS71630</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -6425,269 +6425,269 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MUEL</t>
+          <t>MU1P-C</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MUEL</t>
+          <t>WLS72060</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Naillat</t>
+          <t>MUEL</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>WLS72184</t>
+          <t>MUEL</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Olmedilla</t>
+          <t>Naillat</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>WLS71497</t>
+          <t>WLS72184</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -6818,7 +6818,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Orliac</t>
+          <t>Olmedilla</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -6828,7 +6828,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>WLS72107</t>
+          <t>WLS71497</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -6949,7 +6949,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PEOR-A</t>
+          <t>Orliac</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -6959,7 +6959,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>WLS72070</t>
+          <t>WLS72107</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -7080,7 +7080,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Peregiles I</t>
+          <t>PEOR-A</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -7090,11 +7090,11 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>WLS71604</t>
+          <t>WLS72070</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
@@ -7109,7 +7109,7 @@
         <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="n">
         <v>1</v>
@@ -7130,16 +7130,16 @@
         <v>1</v>
       </c>
       <c r="P51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T51" t="n">
         <v>1</v>
@@ -7148,13 +7148,13 @@
         <v>1</v>
       </c>
       <c r="V51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y51" t="n">
         <v>1</v>
@@ -7163,69 +7163,69 @@
         <v>1</v>
       </c>
       <c r="AA51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Porqueros</t>
+          <t>Notos</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>NADARA_PORQUEROS</t>
+          <t>WLS71604</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
         <v>1</v>
@@ -7234,16 +7234,16 @@
         <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" t="n">
         <v>1</v>
@@ -7261,16 +7261,16 @@
         <v>1</v>
       </c>
       <c r="P52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T52" t="n">
         <v>1</v>
@@ -7279,13 +7279,13 @@
         <v>1</v>
       </c>
       <c r="V52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y52" t="n">
         <v>1</v>
@@ -7294,13 +7294,13 @@
         <v>1</v>
       </c>
       <c r="AA52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD52" t="n">
         <v>0</v>
@@ -7309,72 +7309,72 @@
         <v>0</v>
       </c>
       <c r="AF52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Potrillo</t>
+          <t>Porqueros</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>WLS71413</t>
+          <t>NADARA_PORQUEROS</t>
         </is>
       </c>
       <c r="D53" t="n">
         <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53" t="n">
         <v>1</v>
@@ -7434,10 +7434,10 @@
         <v>1</v>
       </c>
       <c r="AD53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF53" t="n">
         <v>1</v>
@@ -7473,7 +7473,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Procina</t>
+          <t>Potrillo</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -7483,17 +7483,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>WLS72185</t>
+          <t>WLS71413</t>
         </is>
       </c>
       <c r="D54" t="n">
         <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" t="n">
         <v>1</v>
@@ -7604,17 +7604,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Punago-9</t>
+          <t>Procina</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>estaciones.meteo@dekra-industrial.es</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>LIDAR Punago-9</t>
+          <t>WLS72185</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -7702,7 +7702,7 @@
         <v>1</v>
       </c>
       <c r="AF55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG55" t="n">
         <v>1</v>
@@ -7735,138 +7735,138 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Punago-9_2</t>
+          <t>Punago-9</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>estaciones.meteo@dekra-industrial.es</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>WLS71502</t>
+          <t>LIDAR Punago-9</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF56" t="n">
         <v>0</v>
       </c>
       <c r="AG56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Punta del viento 1 : mag 1</t>
+          <t>Punago-9_2</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -7876,259 +7876,259 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Punta_del_Viento-1</t>
+          <t>WLS71502</t>
         </is>
       </c>
       <c r="D57" t="n">
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U57" t="n">
         <v>0</v>
       </c>
       <c r="V57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Ralea III</t>
+          <t>Punta del viento 1 : mag 1</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>WLS71631</t>
+          <t>Punta_del_Viento-1</t>
         </is>
       </c>
       <c r="D58" t="n">
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U58" t="n">
         <v>0</v>
       </c>
       <c r="V58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>REVA-A</t>
+          <t>Ralea III</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -8138,138 +8138,138 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>WLS72024</t>
+          <t>WLS71631</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Rochefort</t>
+          <t>REVA-A</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Rochefort-Montjoyer</t>
+          <t>WLS72024</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -8390,17 +8390,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Saint-Vincent-Jalmoutiers</t>
+          <t>Rochefort</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>WLS72183</t>
+          <t>Rochefort-Montjoyer</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -8521,7 +8521,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Salsola</t>
+          <t>Saint-Vincent-Jalmoutiers</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -8531,7 +8531,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>WLS72188</t>
+          <t>WLS72183</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -8619,40 +8619,40 @@
         <v>1</v>
       </c>
       <c r="AF62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SCHMIEDEHAUSEN</t>
+          <t>Salsola</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -8662,7 +8662,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>WLS71609</t>
+          <t>WLS72188</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -8741,49 +8741,49 @@
         <v>1</v>
       </c>
       <c r="AC63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE63" t="n">
         <v>1</v>
       </c>
       <c r="AF63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SerraJoni 30</t>
+          <t>SCHMIEDEHAUSEN</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -8793,7 +8793,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>WLS72088</t>
+          <t>WLS71609</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -8872,10 +8872,10 @@
         <v>1</v>
       </c>
       <c r="AC64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE64" t="n">
         <v>1</v>
@@ -8914,7 +8914,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>SNA2-A</t>
+          <t>SerraJoni 30</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -8924,7 +8924,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>WLS72067</t>
+          <t>WLS72088</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -9045,7 +9045,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SNA3-A</t>
+          <t>SNA2-A</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -9055,7 +9055,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>WLS72113</t>
+          <t>WLS72067</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -9140,10 +9140,10 @@
         <v>1</v>
       </c>
       <c r="AE66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG66" t="n">
         <v>1</v>
@@ -9176,7 +9176,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Soltau</t>
+          <t>SNA3-A</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -9186,7 +9186,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>WLS71629</t>
+          <t>WLS72113</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -9271,10 +9271,10 @@
         <v>1</v>
       </c>
       <c r="AE67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG67" t="n">
         <v>1</v>
@@ -9307,7 +9307,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Spartivento</t>
+          <t>Soltau</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -9317,7 +9317,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>WLS72321</t>
+          <t>WLS71629</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -9438,21 +9438,21 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Spence1</t>
+          <t>Spartivento</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SPENCE1</t>
+          <t>WLS72321</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
@@ -9569,21 +9569,21 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Tablado-TP_a</t>
+          <t>Spence1</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>WLS72115</t>
+          <t>SPENCE1</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
@@ -9700,17 +9700,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TM Olmillos_1</t>
+          <t>Tablado-TP_a</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>estaciones.meteo@dekra-industrial.es</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Olmillos_1</t>
+          <t>WLS72115</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -9831,17 +9831,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Tort</t>
+          <t>TM Olmillos_1</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>estaciones.meteo@dekra-industrial.es</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Tortoles Esqueva</t>
+          <t>Olmillos_1</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -9863,7 +9863,7 @@
         <v>1</v>
       </c>
       <c r="J72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72" t="n">
         <v>1</v>
@@ -9962,17 +9962,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>URKP-A</t>
+          <t>Tort</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>WLS72216</t>
+          <t>Tortoles Esqueva</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -9994,7 +9994,7 @@
         <v>1</v>
       </c>
       <c r="J73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73" t="n">
         <v>1</v>
@@ -10093,17 +10093,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Valle_de_Navarra_Lidar_2A</t>
+          <t>URKP-A</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>LIDAR Valle_Navarra-2A</t>
+          <t>WLS72216</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -10131,79 +10131,79 @@
         <v>1</v>
       </c>
       <c r="L74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK74" t="n">
         <v>1</v>
@@ -10224,17 +10224,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Valle de Navarra 2A</t>
+          <t>Valle_de_Navarra_Lidar_2A</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>WLS71494</t>
+          <t>LIDAR Valle_Navarra-2A</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -10262,79 +10262,79 @@
         <v>1</v>
       </c>
       <c r="L75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK75" t="n">
         <v>1</v>
@@ -10355,7 +10355,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Villa de Pouca-10</t>
+          <t>Valle de Navarra 2A</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -10365,7 +10365,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>WLS71518</t>
+          <t>WLS71494</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -10486,7 +10486,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Villalube 6B</t>
+          <t>Villa de Pouca-10</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -10496,7 +10496,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>WLS71499</t>
+          <t>WLS71518</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -10617,17 +10617,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Villalube_Lidar_6A_2</t>
+          <t>Villalube 6B</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>emailrelay@konectgds.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>LIDAR Villalube-6A</t>
+          <t>WLS71499</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -10649,7 +10649,7 @@
         <v>1</v>
       </c>
       <c r="J78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78" t="n">
         <v>1</v>
@@ -10667,79 +10667,79 @@
         <v>1</v>
       </c>
       <c r="P78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO78" t="n">
         <v>1</v>
@@ -10748,54 +10748,54 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>WLS71627</t>
+          <t>Villalube_Lidar_6A_2</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>emailrelay@konectgds.com</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>WLS71627</t>
+          <t>LIDAR Villalube-6A</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" t="n">
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P79" t="n">
         <v>0</v>
@@ -10873,23 +10873,23 @@
         <v>0</v>
       </c>
       <c r="AO79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>WLS7-254; Dekra</t>
+          <t>WLS71627</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info-254</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>WLS7-254</t>
+          <t>WLS71627</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -11010,42 +11010,42 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Zagrodno</t>
+          <t>WLS7-254; Dekra</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>windcubeinsights@vaisala.info</t>
+          <t>windcubeinsights@vaisala.info-254</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>WLS72266</t>
+          <t>WLS7-254</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L81" t="n">
         <v>0</v>
@@ -11057,61 +11057,61 @@
         <v>0</v>
       </c>
       <c r="O81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH81" t="n">
         <v>0</v>
@@ -11120,28 +11120,28 @@
         <v>0</v>
       </c>
       <c r="AJ81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Zarzón</t>
+          <t>Zagrodno</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>WLS71446</t>
+          <t>WLS72266</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -11179,13 +11179,13 @@
         <v>1</v>
       </c>
       <c r="L82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O82" t="n">
         <v>1</v>
@@ -11245,10 +11245,10 @@
         <v>1</v>
       </c>
       <c r="AH82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ82" t="n">
         <v>1</v>
@@ -11272,17 +11272,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Zx300 Unit 1148; Almazán 4B</t>
+          <t>Zarzón</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>status@support.zxlidars.com</t>
+          <t>windcubeinsights@vaisala.info</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1148</t>
+          <t>WLS71446</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -11403,7 +11403,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Zx300 Unit 1171; VilaPouca 15</t>
+          <t>Zx300 Unit 1148; Almazán 4B</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -11413,7 +11413,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1171</t>
+          <t>1148</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -11534,7 +11534,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Zx300 Unit 1189; Ayora 1</t>
+          <t>Zx300 Unit 1171; VilaPouca 15</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -11544,7 +11544,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1189</t>
+          <t>1171</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -11665,7 +11665,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Zx300 Unit 1198; Villalube 7</t>
+          <t>Zx300 Unit 1189; Ayora 1</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -11675,7 +11675,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1198</t>
+          <t>1189</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -11796,136 +11796,267 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>Zx300 Unit 1198; Villalube 7</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>status@support.zxlidars.com</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>1198</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" t="n">
+        <v>1</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="n">
+        <v>1</v>
+      </c>
+      <c r="K87" t="n">
+        <v>1</v>
+      </c>
+      <c r="L87" t="n">
+        <v>1</v>
+      </c>
+      <c r="M87" t="n">
+        <v>1</v>
+      </c>
+      <c r="N87" t="n">
+        <v>1</v>
+      </c>
+      <c r="O87" t="n">
+        <v>1</v>
+      </c>
+      <c r="P87" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>1</v>
+      </c>
+      <c r="R87" t="n">
+        <v>1</v>
+      </c>
+      <c r="S87" t="n">
+        <v>1</v>
+      </c>
+      <c r="T87" t="n">
+        <v>1</v>
+      </c>
+      <c r="U87" t="n">
+        <v>1</v>
+      </c>
+      <c r="V87" t="n">
+        <v>1</v>
+      </c>
+      <c r="W87" t="n">
+        <v>1</v>
+      </c>
+      <c r="X87" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y87" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>Zx300 Unit 1611; BetaWind</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>status@support.zxlidars.com</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>1611</t>
         </is>
       </c>
-      <c r="D87" t="n">
-        <v>1</v>
-      </c>
-      <c r="E87" t="n">
-        <v>1</v>
-      </c>
-      <c r="F87" t="n">
-        <v>1</v>
-      </c>
-      <c r="G87" t="n">
-        <v>1</v>
-      </c>
-      <c r="H87" t="n">
-        <v>1</v>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="n">
-        <v>1</v>
-      </c>
-      <c r="K87" t="n">
-        <v>1</v>
-      </c>
-      <c r="L87" t="n">
-        <v>1</v>
-      </c>
-      <c r="M87" t="n">
-        <v>1</v>
-      </c>
-      <c r="N87" t="n">
-        <v>1</v>
-      </c>
-      <c r="O87" t="n">
-        <v>1</v>
-      </c>
-      <c r="P87" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q87" t="n">
-        <v>1</v>
-      </c>
-      <c r="R87" t="n">
-        <v>1</v>
-      </c>
-      <c r="S87" t="n">
-        <v>1</v>
-      </c>
-      <c r="T87" t="n">
-        <v>1</v>
-      </c>
-      <c r="U87" t="n">
-        <v>1</v>
-      </c>
-      <c r="V87" t="n">
-        <v>1</v>
-      </c>
-      <c r="W87" t="n">
-        <v>1</v>
-      </c>
-      <c r="X87" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y87" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN87" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO87" t="n">
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
+      <c r="E88" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" t="n">
+        <v>1</v>
+      </c>
+      <c r="G88" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" t="n">
+        <v>1</v>
+      </c>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="n">
+        <v>1</v>
+      </c>
+      <c r="K88" t="n">
+        <v>1</v>
+      </c>
+      <c r="L88" t="n">
+        <v>1</v>
+      </c>
+      <c r="M88" t="n">
+        <v>1</v>
+      </c>
+      <c r="N88" t="n">
+        <v>1</v>
+      </c>
+      <c r="O88" t="n">
+        <v>1</v>
+      </c>
+      <c r="P88" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>1</v>
+      </c>
+      <c r="R88" t="n">
+        <v>1</v>
+      </c>
+      <c r="S88" t="n">
+        <v>1</v>
+      </c>
+      <c r="T88" t="n">
+        <v>1</v>
+      </c>
+      <c r="U88" t="n">
+        <v>1</v>
+      </c>
+      <c r="V88" t="n">
+        <v>1</v>
+      </c>
+      <c r="W88" t="n">
+        <v>1</v>
+      </c>
+      <c r="X88" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y88" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO88" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D87">
+  <conditionalFormatting sqref="D2:D88">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11933,7 +12064,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E87">
+  <conditionalFormatting sqref="E2:E88">
     <cfRule type="cellIs" priority="3" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11941,7 +12072,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F87">
+  <conditionalFormatting sqref="F2:F88">
     <cfRule type="cellIs" priority="5" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11949,7 +12080,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G87">
+  <conditionalFormatting sqref="G2:G88">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11957,7 +12088,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H87">
+  <conditionalFormatting sqref="H2:H88">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11965,7 +12096,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I87">
+  <conditionalFormatting sqref="I2:I88">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11973,7 +12104,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J87">
+  <conditionalFormatting sqref="J2:J88">
     <cfRule type="cellIs" priority="13" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11981,7 +12112,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K87">
+  <conditionalFormatting sqref="K2:K88">
     <cfRule type="cellIs" priority="15" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11989,7 +12120,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L87">
+  <conditionalFormatting sqref="L2:L88">
     <cfRule type="cellIs" priority="17" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -11997,7 +12128,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M87">
+  <conditionalFormatting sqref="M2:M88">
     <cfRule type="cellIs" priority="19" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12005,7 +12136,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N87">
+  <conditionalFormatting sqref="N2:N88">
     <cfRule type="cellIs" priority="21" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12013,7 +12144,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O87">
+  <conditionalFormatting sqref="O2:O88">
     <cfRule type="cellIs" priority="23" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12021,7 +12152,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P87">
+  <conditionalFormatting sqref="P2:P88">
     <cfRule type="cellIs" priority="25" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12029,7 +12160,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q87">
+  <conditionalFormatting sqref="Q2:Q88">
     <cfRule type="cellIs" priority="27" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12037,7 +12168,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R87">
+  <conditionalFormatting sqref="R2:R88">
     <cfRule type="cellIs" priority="29" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12045,7 +12176,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S87">
+  <conditionalFormatting sqref="S2:S88">
     <cfRule type="cellIs" priority="31" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12053,7 +12184,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T87">
+  <conditionalFormatting sqref="T2:T88">
     <cfRule type="cellIs" priority="33" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12061,7 +12192,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U87">
+  <conditionalFormatting sqref="U2:U88">
     <cfRule type="cellIs" priority="35" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12069,7 +12200,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V87">
+  <conditionalFormatting sqref="V2:V88">
     <cfRule type="cellIs" priority="37" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12077,7 +12208,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W87">
+  <conditionalFormatting sqref="W2:W88">
     <cfRule type="cellIs" priority="39" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12085,7 +12216,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X87">
+  <conditionalFormatting sqref="X2:X88">
     <cfRule type="cellIs" priority="41" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12093,7 +12224,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y87">
+  <conditionalFormatting sqref="Y2:Y88">
     <cfRule type="cellIs" priority="43" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12101,7 +12232,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z87">
+  <conditionalFormatting sqref="Z2:Z88">
     <cfRule type="cellIs" priority="45" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12109,7 +12240,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA87">
+  <conditionalFormatting sqref="AA2:AA88">
     <cfRule type="cellIs" priority="47" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12117,7 +12248,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB87">
+  <conditionalFormatting sqref="AB2:AB88">
     <cfRule type="cellIs" priority="49" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12125,7 +12256,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC87">
+  <conditionalFormatting sqref="AC2:AC88">
     <cfRule type="cellIs" priority="51" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12133,7 +12264,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD87">
+  <conditionalFormatting sqref="AD2:AD88">
     <cfRule type="cellIs" priority="53" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12141,7 +12272,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE87">
+  <conditionalFormatting sqref="AE2:AE88">
     <cfRule type="cellIs" priority="55" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12149,7 +12280,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF2:AF87">
+  <conditionalFormatting sqref="AF2:AF88">
     <cfRule type="cellIs" priority="57" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12157,7 +12288,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG87">
+  <conditionalFormatting sqref="AG2:AG88">
     <cfRule type="cellIs" priority="59" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12165,7 +12296,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH87">
+  <conditionalFormatting sqref="AH2:AH88">
     <cfRule type="cellIs" priority="61" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12173,7 +12304,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI2:AI87">
+  <conditionalFormatting sqref="AI2:AI88">
     <cfRule type="cellIs" priority="63" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12181,7 +12312,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2:AJ87">
+  <conditionalFormatting sqref="AJ2:AJ88">
     <cfRule type="cellIs" priority="65" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12189,7 +12320,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK87">
+  <conditionalFormatting sqref="AK2:AK88">
     <cfRule type="cellIs" priority="67" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12197,7 +12328,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL2:AL87">
+  <conditionalFormatting sqref="AL2:AL88">
     <cfRule type="cellIs" priority="69" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12205,7 +12336,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM87">
+  <conditionalFormatting sqref="AM2:AM88">
     <cfRule type="cellIs" priority="71" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12213,7 +12344,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AN2:AN87">
+  <conditionalFormatting sqref="AN2:AN88">
     <cfRule type="cellIs" priority="73" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>
@@ -12221,7 +12352,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO2:AO87">
+  <conditionalFormatting sqref="AO2:AO88">
     <cfRule type="cellIs" priority="75" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>1</formula>
     </cfRule>

</xml_diff>